<commit_message>
fixed datetime issue again with v2
</commit_message>
<xml_diff>
--- a/data/data2.xlsx
+++ b/data/data2.xlsx
@@ -15,17 +15,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -104,18 +109,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
@@ -125,20 +136,14 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,95 +518,97 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="0.7192857142857143" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
-    <col width="28.14785714285714" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
-    <col width="17.43357142857143" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="28.005" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="51.57642857142857" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
-    <col width="91.005" bestFit="1" customWidth="1" style="9" min="6" max="6"/>
-    <col width="195.8621428571429" bestFit="1" customWidth="1" style="9" min="7" max="7"/>
-    <col width="18.43357142857143" bestFit="1" customWidth="1" style="9" min="8" max="8"/>
-    <col width="15.71928571428571" bestFit="1" customWidth="1" style="11" min="9" max="9"/>
+    <col width="0.7192857142857143" bestFit="1" customWidth="1" style="11" min="1" max="1"/>
+    <col width="28.14785714285714" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="17.43357142857143" bestFit="1" customWidth="1" style="11" min="3" max="3"/>
+    <col width="28.005" bestFit="1" customWidth="1" style="11" min="4" max="4"/>
+    <col width="51.57642857142857" bestFit="1" customWidth="1" style="11" min="5" max="5"/>
+    <col width="91.005" bestFit="1" customWidth="1" style="11" min="6" max="6"/>
+    <col width="195.8621428571429" bestFit="1" customWidth="1" style="11" min="7" max="7"/>
+    <col width="18.43357142857143" bestFit="1" customWidth="1" style="11" min="8" max="8"/>
+    <col width="15.71928571428571" bestFit="1" customWidth="1" style="13" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" s="12" t="inlineStr">
+    <row r="1" ht="21" customHeight="1">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Date/Time local</t>
         </is>
       </c>
-      <c r="B1" s="13" t="inlineStr">
+      <c r="B1" s="15" t="inlineStr">
         <is>
           <t>Date/Time MPNET</t>
         </is>
       </c>
-      <c r="C1" s="12" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>MITRE Tactic</t>
         </is>
       </c>
-      <c r="D1" s="12" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Source Hostname/IP</t>
         </is>
       </c>
-      <c r="E1" s="12" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Target Hostname/IP</t>
         </is>
       </c>
-      <c r="F1" s="12" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
       </c>
-      <c r="G1" s="12" t="inlineStr">
+      <c r="G1" s="14" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="H1" s="12" t="inlineStr">
+      <c r="H1" s="14" t="inlineStr">
         <is>
           <t>Operator</t>
         </is>
       </c>
-      <c r="I1" s="14" t="inlineStr">
+      <c r="I1" s="16" t="inlineStr">
         <is>
           <t>Attack Chain</t>
         </is>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="9" t="inlineStr"/>
-      <c r="B2" s="15" t="n">
-        <v>45396.94583333333</v>
-      </c>
-      <c r="C2" s="9" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr"/>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>04/14/2024, 2242</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
         <is>
           <t>C2</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
+      <c r="D2" s="11" t="inlineStr">
         <is>
           <t>8.29.22.50</t>
         </is>
       </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
         <is>
           <t>172.217.25.50</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>googleService.exe C2 Beacon (cdn.google.com)</t>
         </is>
       </c>
-      <c r="G2" s="9" t="inlineStr">
+      <c r="G2" s="11" t="inlineStr">
         <is>
           <t>over 443/https</t>
         </is>
       </c>
-      <c r="H2" s="9" t="inlineStr">
+      <c r="H2" s="11" t="inlineStr">
         <is>
           <t>wermeling</t>
         </is>
@@ -611,32 +618,34 @@
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="9" t="inlineStr"/>
-      <c r="B3" s="16" t="n">
-        <v>45396.92708333334</v>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr"/>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>04/14/2024, 2215</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
         <is>
           <t>Exfiltration</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
+      <c r="D3" s="11" t="inlineStr">
         <is>
           <t>207.228.7.52</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" s="11" t="inlineStr">
         <is>
           <t>172.217.25.50</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" s="11" t="inlineStr">
         <is>
           <t>Likely exfiltration seen from .52 to 172.217.25.50 (cdn.google.com)</t>
         </is>
       </c>
-      <c r="G3" s="9" t="inlineStr"/>
-      <c r="H3" s="9" t="inlineStr">
+      <c r="G3" s="11" t="inlineStr"/>
+      <c r="H3" s="11" t="inlineStr">
         <is>
           <t>castillo</t>
         </is>
@@ -646,32 +655,34 @@
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="9" t="inlineStr"/>
-      <c r="B4" s="15" t="n">
-        <v>45396.86666666667</v>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr"/>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>04/14/2024, 2048</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
         <is>
           <t>Persistence</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
+      <c r="D4" s="11" t="inlineStr">
         <is>
           <t>rom-nix-1</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr"/>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="E4" s="11" t="inlineStr"/>
+      <c r="F4" s="11" t="inlineStr">
         <is>
           <t>myssql user creation</t>
         </is>
       </c>
-      <c r="G4" s="9" t="inlineStr">
+      <c r="G4" s="11" t="inlineStr">
         <is>
           <t>mispelled name, passwd assigned, has bash shell access, all inconsistent with a service account</t>
         </is>
       </c>
-      <c r="H4" s="9" t="inlineStr">
+      <c r="H4" s="11" t="inlineStr">
         <is>
           <t>gary</t>
         </is>
@@ -681,36 +692,38 @@
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="9" t="inlineStr"/>
-      <c r="B5" s="15" t="n">
-        <v>45396.80347222222</v>
-      </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr"/>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>04/14/2024, 1917</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>C2</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
+      <c r="D5" s="11" t="inlineStr">
         <is>
           <t>207.228.76.9 (rom-kerberos)</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>172.217.25.50</t>
         </is>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="11" t="inlineStr">
         <is>
           <t>Traffic spike in unknownkrb server C2 Beacon</t>
         </is>
       </c>
-      <c r="G5" s="9" t="inlineStr">
+      <c r="G5" s="11" t="inlineStr">
         <is>
           <t>over 443/https</t>
         </is>
       </c>
-      <c r="H5" s="9" t="inlineStr">
+      <c r="H5" s="11" t="inlineStr">
         <is>
           <t>wermeling</t>
         </is>
@@ -720,36 +733,38 @@
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="9" t="inlineStr"/>
-      <c r="B6" s="15" t="n">
-        <v>45396.79930555556</v>
-      </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>04/14/2024, 1911</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>C2</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
+      <c r="D6" s="11" t="inlineStr">
         <is>
           <t>207.228.76.9 (rom-kerberos)</t>
         </is>
       </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>172.217.25.50</t>
         </is>
       </c>
-      <c r="F6" s="9" t="inlineStr">
+      <c r="F6" s="11" t="inlineStr">
         <is>
           <t>unknown krb server C2 Beacon</t>
         </is>
       </c>
-      <c r="G6" s="9" t="inlineStr">
+      <c r="G6" s="11" t="inlineStr">
         <is>
           <t>over 443/https</t>
         </is>
       </c>
-      <c r="H6" s="9" t="inlineStr">
+      <c r="H6" s="11" t="inlineStr">
         <is>
           <t>wermeling</t>
         </is>
@@ -759,36 +774,38 @@
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="9" t="inlineStr"/>
-      <c r="B7" s="15" t="n">
-        <v>45396.79305555556</v>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="A7" s="11" t="inlineStr"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>04/14/2024, 1902</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>Execution</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
+      <c r="D7" s="11" t="inlineStr">
         <is>
           <t>207.228.76.9 (rom-kerberos)</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>152.58.88.106</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" s="11" t="inlineStr">
         <is>
           <t>Download/execution of apache2.elf from techspaceinfo.com to the rom-kerberos</t>
         </is>
       </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="G7" s="11" t="inlineStr">
         <is>
           <t>over 8443/https</t>
         </is>
       </c>
-      <c r="H7" s="9" t="inlineStr">
+      <c r="H7" s="11" t="inlineStr">
         <is>
           <t>castillo</t>
         </is>
@@ -798,36 +815,38 @@
       </c>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="9" t="inlineStr"/>
-      <c r="B8" s="15" t="n">
-        <v>45396.79166666666</v>
-      </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr"/>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>04/14/2024, 1900</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="inlineStr">
         <is>
           <t>C2</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
+      <c r="D8" s="11" t="inlineStr">
         <is>
           <t>207.228.7.52</t>
         </is>
       </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="E8" s="11" t="inlineStr">
         <is>
           <t>175.217.25.50</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="F8" s="11" t="inlineStr">
         <is>
           <t>googleService.exe C2 Beacon (cdn.google.com)</t>
         </is>
       </c>
-      <c r="G8" s="9" t="inlineStr">
+      <c r="G8" s="11" t="inlineStr">
         <is>
           <t>over 443/https</t>
         </is>
       </c>
-      <c r="H8" s="9" t="inlineStr">
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>wermeling</t>
         </is>
@@ -837,36 +856,38 @@
       </c>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="9" t="inlineStr"/>
-      <c r="B9" s="15" t="n">
-        <v>45395.79722222222</v>
-      </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="A9" s="11" t="inlineStr"/>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>04/13/2024, 1908</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
         <is>
           <t>Lateral Movement</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
+      <c r="D9" s="11" t="inlineStr">
         <is>
           <t>8.29.22.51</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>207.228.7.51, 207.228.7.59, 207.228.76.3, 8.29.168.2</t>
         </is>
       </c>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="11" t="inlineStr">
         <is>
           <t>SMB File Transfer of googleService.exe &amp; BIT430E.tmp</t>
         </is>
       </c>
-      <c r="G9" s="9" t="inlineStr">
+      <c r="G9" s="11" t="inlineStr">
         <is>
           <t>googleService.exe moved from achaeans to romans, BIT430E.tmp moved intra-domain within achaeans</t>
         </is>
       </c>
-      <c r="H9" s="9" t="inlineStr">
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>wermeling/castillo</t>
         </is>
@@ -876,36 +897,38 @@
       </c>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="9" t="inlineStr"/>
-      <c r="B10" s="15" t="n">
-        <v>45395.74375</v>
-      </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="A10" s="11" t="inlineStr"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>04/13/2024, 1751</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>Execution</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
+      <c r="D10" s="11" t="inlineStr">
         <is>
           <t>8.29.22.51</t>
         </is>
       </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="E10" s="11" t="inlineStr">
         <is>
           <t>192.58.88.106</t>
         </is>
       </c>
-      <c r="F10" s="9" t="inlineStr">
+      <c r="F10" s="11" t="inlineStr">
         <is>
           <t>Download/execution of googleService.exe</t>
         </is>
       </c>
-      <c r="G10" s="9" t="inlineStr">
+      <c r="G10" s="11" t="inlineStr">
         <is>
           <t>techspaceinfo[.]com (192.58.88.106)</t>
         </is>
       </c>
-      <c r="H10" s="9" t="inlineStr">
+      <c r="H10" s="11" t="inlineStr">
         <is>
           <t>wermeling/castillo</t>
         </is>
@@ -915,36 +938,38 @@
       </c>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="9" t="inlineStr"/>
-      <c r="B11" s="15" t="n">
-        <v>45394.90625</v>
-      </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="A11" s="11" t="inlineStr"/>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>04/12/2024, 2145</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="inlineStr">
         <is>
           <t>Discovery</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
+      <c r="D11" s="11" t="inlineStr">
         <is>
           <t>101.13.240.46</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="E11" s="11" t="inlineStr">
         <is>
           <t>8.29.22.2, 8.29.22.5</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="11" t="inlineStr">
         <is>
           <t>Nmap Discovery</t>
         </is>
       </c>
-      <c r="G11" s="9" t="inlineStr">
+      <c r="G11" s="11" t="inlineStr">
         <is>
           <t>Discovery of 80 (.2) &amp; 445/5985 (.5)</t>
         </is>
       </c>
-      <c r="H11" s="9" t="inlineStr">
+      <c r="H11" s="11" t="inlineStr">
         <is>
           <t>jonathas</t>
         </is>
@@ -954,36 +979,38 @@
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="9" t="inlineStr"/>
-      <c r="B12" s="15" t="n">
-        <v>45394.83541666667</v>
-      </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="A12" s="11" t="inlineStr"/>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>04/12/2024, 2003</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="inlineStr">
         <is>
           <t>Lateral Movement</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
+      <c r="D12" s="11" t="inlineStr">
         <is>
           <t>8.29.22.59</t>
         </is>
       </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="E12" s="11" t="inlineStr">
         <is>
           <t>8.29.168.5</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">googleService.exe spawned traffic to 8.29.168.5 (ACH-DC) </t>
         </is>
       </c>
-      <c r="G12" s="9" t="inlineStr">
+      <c r="G12" s="11" t="inlineStr">
         <is>
           <t>Port 49666 was used</t>
         </is>
       </c>
-      <c r="H12" s="9" t="inlineStr">
+      <c r="H12" s="11" t="inlineStr">
         <is>
           <t>wermeling, colon</t>
         </is>
@@ -993,32 +1020,34 @@
       </c>
     </row>
     <row r="13" ht="19.5" customHeight="1">
-      <c r="A13" s="9" t="inlineStr"/>
-      <c r="B13" s="15" t="n">
-        <v>45394.81527777778</v>
-      </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="A13" s="11" t="inlineStr"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>04/12/2024, 1934</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="inlineStr">
         <is>
           <t>Initial Access</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
+      <c r="D13" s="11" t="inlineStr">
         <is>
           <t>192.58.88.106</t>
         </is>
       </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>8.29.168.2</t>
         </is>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="11" t="inlineStr">
         <is>
           <t>Spearphishing campaign against 20+ users</t>
         </is>
       </c>
-      <c r="G13" s="8" t="inlineStr"/>
-      <c r="H13" s="9" t="inlineStr">
+      <c r="G13" s="11" t="inlineStr"/>
+      <c r="H13" s="11" t="inlineStr">
         <is>
           <t>wermeling</t>
         </is>
@@ -1028,156 +1057,156 @@
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
-      <c r="A14" s="9" t="inlineStr"/>
-      <c r="B14" s="7" t="inlineStr">
-        <is>
-          <t>04/12/2024, 1921</t>
-        </is>
-      </c>
-      <c r="C14" s="8" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr"/>
+      <c r="B14" s="8" t="inlineStr">
+        <is>
+          <t>04/14/2024, 1920</t>
+        </is>
+      </c>
+      <c r="C14" s="9" t="inlineStr">
         <is>
           <t>Initial Access</t>
         </is>
       </c>
-      <c r="D14" s="8" t="inlineStr">
+      <c r="D14" s="9" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="E14" s="9" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="F14" s="8" t="inlineStr">
+      <c r="F14" s="9" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="G14" s="8" t="inlineStr">
+      <c r="G14" s="9" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="H14" s="8" t="inlineStr">
+      <c r="H14" s="9" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="I14" s="6" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="9" t="n"/>
+      <c r="A15" s="11" t="n"/>
       <c r="B15" s="7" t="n"/>
-      <c r="C15" s="8" t="inlineStr"/>
-      <c r="D15" s="8" t="inlineStr"/>
-      <c r="E15" s="8" t="inlineStr"/>
-      <c r="F15" s="8" t="inlineStr"/>
-      <c r="G15" s="9" t="n"/>
-      <c r="H15" s="8" t="inlineStr"/>
+      <c r="C15" s="11" t="n"/>
+      <c r="D15" s="11" t="n"/>
+      <c r="E15" s="11" t="n"/>
+      <c r="F15" s="11" t="n"/>
+      <c r="G15" s="11" t="n"/>
+      <c r="H15" s="11" t="n"/>
       <c r="I15" s="6" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="9" t="n"/>
+      <c r="A16" s="11" t="n"/>
       <c r="B16" s="7" t="n"/>
-      <c r="C16" s="9" t="n"/>
-      <c r="D16" s="9" t="n"/>
-      <c r="E16" s="9" t="n"/>
-      <c r="F16" s="9" t="n"/>
-      <c r="G16" s="9" t="n"/>
-      <c r="H16" s="9" t="n"/>
+      <c r="C16" s="11" t="n"/>
+      <c r="D16" s="11" t="n"/>
+      <c r="E16" s="11" t="n"/>
+      <c r="F16" s="11" t="n"/>
+      <c r="G16" s="11" t="n"/>
+      <c r="H16" s="11" t="n"/>
       <c r="I16" s="6" t="n"/>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="9" t="n"/>
+      <c r="A17" s="11" t="n"/>
       <c r="B17" s="7" t="n"/>
-      <c r="C17" s="9" t="n"/>
-      <c r="D17" s="9" t="n"/>
-      <c r="E17" s="9" t="n"/>
-      <c r="F17" s="9" t="n"/>
-      <c r="G17" s="9" t="n"/>
-      <c r="H17" s="9" t="n"/>
+      <c r="C17" s="11" t="n"/>
+      <c r="D17" s="11" t="n"/>
+      <c r="E17" s="11" t="n"/>
+      <c r="F17" s="11" t="n"/>
+      <c r="G17" s="11" t="n"/>
+      <c r="H17" s="11" t="n"/>
       <c r="I17" s="6" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="9" t="n"/>
+      <c r="A18" s="11" t="n"/>
       <c r="B18" s="7" t="n"/>
-      <c r="C18" s="9" t="n"/>
-      <c r="D18" s="9" t="n"/>
-      <c r="E18" s="9" t="n"/>
-      <c r="F18" s="9" t="n"/>
-      <c r="G18" s="9" t="n"/>
-      <c r="H18" s="9" t="n"/>
+      <c r="C18" s="11" t="n"/>
+      <c r="D18" s="11" t="n"/>
+      <c r="E18" s="11" t="n"/>
+      <c r="F18" s="11" t="n"/>
+      <c r="G18" s="11" t="n"/>
+      <c r="H18" s="11" t="n"/>
       <c r="I18" s="6" t="n"/>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="9" t="n"/>
+      <c r="A19" s="11" t="n"/>
       <c r="B19" s="7" t="n"/>
-      <c r="C19" s="9" t="n"/>
-      <c r="D19" s="9" t="n"/>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-      <c r="G19" s="9" t="n"/>
-      <c r="H19" s="9" t="n"/>
+      <c r="C19" s="11" t="n"/>
+      <c r="D19" s="11" t="n"/>
+      <c r="E19" s="11" t="n"/>
+      <c r="F19" s="11" t="n"/>
+      <c r="G19" s="11" t="n"/>
+      <c r="H19" s="11" t="n"/>
       <c r="I19" s="6" t="n"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="9" t="n"/>
+      <c r="A20" s="11" t="n"/>
       <c r="B20" s="7" t="n"/>
-      <c r="C20" s="9" t="n"/>
-      <c r="D20" s="9" t="n"/>
-      <c r="E20" s="9" t="n"/>
-      <c r="F20" s="9" t="n"/>
-      <c r="G20" s="9" t="n"/>
-      <c r="H20" s="9" t="n"/>
+      <c r="C20" s="11" t="n"/>
+      <c r="D20" s="11" t="n"/>
+      <c r="E20" s="11" t="n"/>
+      <c r="F20" s="11" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="11" t="n"/>
       <c r="I20" s="6" t="n"/>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="9" t="n"/>
+      <c r="A21" s="11" t="n"/>
       <c r="B21" s="7" t="n"/>
-      <c r="C21" s="9" t="n"/>
-      <c r="D21" s="9" t="n"/>
-      <c r="E21" s="9" t="n"/>
-      <c r="F21" s="9" t="n"/>
-      <c r="G21" s="9" t="n"/>
-      <c r="H21" s="9" t="n"/>
+      <c r="C21" s="11" t="n"/>
+      <c r="D21" s="11" t="n"/>
+      <c r="E21" s="11" t="n"/>
+      <c r="F21" s="11" t="n"/>
+      <c r="G21" s="11" t="n"/>
+      <c r="H21" s="11" t="n"/>
       <c r="I21" s="6" t="n"/>
     </row>
     <row r="22" ht="19.5" customHeight="1">
-      <c r="A22" s="9" t="n"/>
+      <c r="A22" s="11" t="n"/>
       <c r="B22" s="7" t="n"/>
-      <c r="C22" s="9" t="n"/>
-      <c r="D22" s="9" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-      <c r="G22" s="9" t="n"/>
-      <c r="H22" s="9" t="n"/>
+      <c r="C22" s="11" t="n"/>
+      <c r="D22" s="11" t="n"/>
+      <c r="E22" s="11" t="n"/>
+      <c r="F22" s="11" t="n"/>
+      <c r="G22" s="11" t="n"/>
+      <c r="H22" s="11" t="n"/>
       <c r="I22" s="6" t="n"/>
     </row>
     <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="9" t="n"/>
+      <c r="A23" s="11" t="n"/>
       <c r="B23" s="7" t="n"/>
-      <c r="C23" s="9" t="n"/>
-      <c r="D23" s="9" t="n"/>
-      <c r="E23" s="9" t="n"/>
-      <c r="F23" s="9" t="n"/>
-      <c r="G23" s="9" t="n"/>
-      <c r="H23" s="9" t="n"/>
+      <c r="C23" s="11" t="n"/>
+      <c r="D23" s="11" t="n"/>
+      <c r="E23" s="11" t="n"/>
+      <c r="F23" s="11" t="n"/>
+      <c r="G23" s="11" t="n"/>
+      <c r="H23" s="11" t="n"/>
       <c r="I23" s="6" t="n"/>
     </row>
     <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="9" t="n"/>
+      <c r="A24" s="11" t="n"/>
       <c r="B24" s="7" t="n"/>
-      <c r="C24" s="9" t="n"/>
-      <c r="D24" s="9" t="n"/>
-      <c r="E24" s="9" t="n"/>
-      <c r="F24" s="9" t="n"/>
-      <c r="G24" s="9" t="n"/>
-      <c r="H24" s="9" t="n"/>
+      <c r="C24" s="11" t="n"/>
+      <c r="D24" s="11" t="n"/>
+      <c r="E24" s="11" t="n"/>
+      <c r="F24" s="11" t="n"/>
+      <c r="G24" s="11" t="n"/>
+      <c r="H24" s="11" t="n"/>
       <c r="I24" s="6" t="n"/>
     </row>
   </sheetData>

</xml_diff>